<commit_message>
Progress is on util/PDOSQL.php Line 72.
</commit_message>
<xml_diff>
--- a/_plannings/Gantt chart.xlsx
+++ b/_plannings/Gantt chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>WEEKS</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>- Implementation plan</t>
+  </si>
+  <si>
+    <t>Course E</t>
   </si>
 </sst>
 </file>
@@ -433,6 +436,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -446,13 +456,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -773,67 +776,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="19" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="19" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="19" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="19" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -983,7 +986,7 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1048,7 +1051,7 @@
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1083,7 +1086,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="8"/>
@@ -1116,7 +1119,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="8"/>
@@ -1160,7 +1163,9 @@
         <v>28</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="J9" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1187,8 +1192,12 @@
         <v>32</v>
       </c>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="J10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -1301,7 +1310,7 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="8"/>
@@ -1376,8 +1385,12 @@
       <c r="I17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="J17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1530,7 +1543,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="8"/>
@@ -1611,7 +1624,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="26"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -1655,7 +1668,7 @@
       <c r="U26" s="8"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="19" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="8"/>
@@ -1705,7 +1718,7 @@
       <c r="U28" s="8"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="8"/>
@@ -1755,7 +1768,7 @@
       <c r="U30" s="8"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="19" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="8"/>
@@ -1880,7 +1893,7 @@
       <c r="U35" s="8"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="8"/>

</xml_diff>